<commit_message>
use 'c' for Mackinnon to avoid 'nc' error
</commit_message>
<xml_diff>
--- a/MappingTheFederalReserve'sResponseFunctionWithDirectedAcyclicGraphs/SUR2005-12-31-2008-09-30.xlsx
+++ b/MappingTheFederalReserve'sResponseFunctionWithDirectedAcyclicGraphs/SUR2005-12-31-2008-09-30.xlsx
@@ -22,16 +22,16 @@
     <t>FFR_LF</t>
   </si>
   <si>
+    <t>LF_A</t>
+  </si>
+  <si>
+    <t>LF_FFR</t>
+  </si>
+  <si>
     <t>A_FFR</t>
   </si>
   <si>
     <t>A_LF</t>
-  </si>
-  <si>
-    <t>LF_A</t>
-  </si>
-  <si>
-    <t>LF_FFR</t>
   </si>
   <si>
     <t>params</t>
@@ -426,22 +426,22 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>31.61408023314106</v>
+        <v>31.61408023314126</v>
       </c>
       <c r="C2">
-        <v>2.648915369657083</v>
+        <v>2.648915369657086</v>
       </c>
       <c r="D2">
-        <v>0.006278165067028139</v>
+        <v>-18.7486205613615</v>
       </c>
       <c r="E2">
-        <v>-0.03195948140161898</v>
+        <v>0.3085956916096014</v>
       </c>
       <c r="F2">
-        <v>-18.74862056136149</v>
+        <v>0.006278165067028148</v>
       </c>
       <c r="G2">
-        <v>0.3085956916096013</v>
+        <v>-0.03195948140161897</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -449,22 +449,22 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.003703943600201987</v>
+        <v>0.003703943600201542</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
+        <v>5.687406101628767E-11</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
         <v>0.003703943600202209</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>5.687406101628767E-11</v>
-      </c>
-      <c r="F3">
-        <v>5.687406101628767E-11</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add monthly test with acf plot
</commit_message>
<xml_diff>
--- a/MappingTheFederalReserve'sResponseFunctionWithDirectedAcyclicGraphs/SUR2005-12-31-2008-09-30.xlsx
+++ b/MappingTheFederalReserve'sResponseFunctionWithDirectedAcyclicGraphs/SUR2005-12-31-2008-09-30.xlsx
@@ -16,22 +16,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
+    <t>LF_A</t>
+  </si>
+  <si>
+    <t>LF_FFR</t>
+  </si>
+  <si>
+    <t>FFR_A</t>
+  </si>
+  <si>
+    <t>FFR_LF</t>
+  </si>
+  <si>
     <t>A_FFR</t>
   </si>
   <si>
     <t>A_LF</t>
-  </si>
-  <si>
-    <t>FFR_A</t>
-  </si>
-  <si>
-    <t>FFR_LF</t>
-  </si>
-  <si>
-    <t>LF_A</t>
-  </si>
-  <si>
-    <t>LF_FFR</t>
   </si>
   <si>
     <t>params</t>
@@ -426,22 +426,22 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>0.00627816506702822</v>
+        <v>-18.7486205613612</v>
       </c>
       <c r="C2">
-        <v>-0.03195948140161915</v>
+        <v>0.3085956916096027</v>
       </c>
       <c r="D2">
-        <v>31.61408023314044</v>
+        <v>31.61408023313981</v>
       </c>
       <c r="E2">
-        <v>2.648915369657071</v>
+        <v>2.648915369657066</v>
       </c>
       <c r="F2">
-        <v>-18.74862056136134</v>
+        <v>0.006278165067028211</v>
       </c>
       <c r="G2">
-        <v>0.3085956916096025</v>
+        <v>-0.03195948140161918</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -449,22 +449,22 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.003703943600201764</v>
+        <v>5.687406101628767E-11</v>
       </c>
       <c r="C3">
-        <v>5.687406101628767E-11</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0.003703943600202653</v>
+        <v>0.003703943600203319</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
+        <v>0.003703943600201987</v>
+      </c>
+      <c r="G3">
         <v>5.687406101628767E-11</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>